<commit_message>
pushing browse page progress from night of april 12
</commit_message>
<xml_diff>
--- a/sampleUsers.xlsx
+++ b/sampleUsers.xlsx
@@ -9226,7 +9226,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -9269,12 +9269,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="44">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -9298,6 +9300,7 @@
     <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -9316,6 +9319,7 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -9658,8 +9662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" topLeftCell="A992" workbookViewId="0">
+      <selection activeCell="D1013" sqref="D1013"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
got right panel on browsing page up and running, got rid of iframe, some map panning / list scrolling interactivity, made cart section nicer for profile.html
</commit_message>
<xml_diff>
--- a/sampleUsers.xlsx
+++ b/sampleUsers.xlsx
@@ -9226,7 +9226,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -9271,12 +9271,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="62">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -9301,6 +9319,15 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -9320,6 +9347,15 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -9662,8 +9698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A992" workbookViewId="0">
-      <selection activeCell="D1013" sqref="D1013"/>
+    <sheetView tabSelected="1" topLeftCell="A597" workbookViewId="0">
+      <selection activeCell="D604" sqref="D604"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>